<commit_message>
Add Branch Prediction Unit
</commit_message>
<xml_diff>
--- a/MIPS ISA.xlsx
+++ b/MIPS ISA.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="28526"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="26327"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\moame\Downloads\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\New folder\MIPS32_Pipelined_Processor\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0DFFFB3E-401A-4D50-954F-7E107C34C9D2}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C4691D42-CFBA-4294-BAAE-E94A21323BAB}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -27,7 +27,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="252" uniqueCount="226">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="244" uniqueCount="219">
   <si>
     <t xml:space="preserve">Opcode </t>
   </si>
@@ -693,27 +693,6 @@
   </si>
   <si>
     <t>[rt] = [rd]/[rd] = [rt]</t>
-  </si>
-  <si>
-    <t xml:space="preserve">001100 (12) </t>
-  </si>
-  <si>
-    <t xml:space="preserve">syscall </t>
-  </si>
-  <si>
-    <t xml:space="preserve">system call </t>
-  </si>
-  <si>
-    <t>system call exception</t>
-  </si>
-  <si>
-    <t xml:space="preserve">001101 (13) </t>
-  </si>
-  <si>
-    <t xml:space="preserve">break </t>
-  </si>
-  <si>
-    <t>break exception</t>
   </si>
 </sst>
 </file>
@@ -872,7 +851,22 @@
   </cellStyles>
   <dxfs count="12">
     <dxf>
-      <alignment horizontal="left" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+      <alignment horizontal="left" vertical="center" textRotation="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <alignment horizontal="left" vertical="center" textRotation="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <alignment horizontal="left" vertical="center" textRotation="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <alignment horizontal="left" vertical="center" textRotation="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <alignment horizontal="left" vertical="center" textRotation="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <alignment horizontal="left" vertical="center" textRotation="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
     </dxf>
     <dxf>
       <alignment horizontal="left" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
@@ -890,22 +884,7 @@
       <alignment horizontal="left" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
     </dxf>
     <dxf>
-      <alignment horizontal="left" vertical="center" textRotation="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
-    <dxf>
-      <alignment horizontal="left" vertical="center" textRotation="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
-    <dxf>
-      <alignment horizontal="left" vertical="center" textRotation="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
-    <dxf>
-      <alignment horizontal="left" vertical="center" textRotation="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
-    <dxf>
-      <alignment horizontal="left" vertical="center" textRotation="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
-    <dxf>
-      <alignment horizontal="left" vertical="center" textRotation="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+      <alignment horizontal="left" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
     </dxf>
   </dxfs>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
@@ -1063,26 +1042,26 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{0D33F033-7401-4F1F-8987-FB63CD7DF6BC}" name="Table1" displayName="Table1" ref="A1:D27" totalsRowShown="0" headerRowDxfId="5" dataDxfId="4">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{0D33F033-7401-4F1F-8987-FB63CD7DF6BC}" name="Table1" displayName="Table1" ref="A1:D27" totalsRowShown="0" headerRowDxfId="11" dataDxfId="10">
   <autoFilter ref="A1:D27" xr:uid="{0D33F033-7401-4F1F-8987-FB63CD7DF6BC}"/>
   <tableColumns count="4">
-    <tableColumn id="1" xr3:uid="{6F141741-2C51-4220-AFC7-E5871EC6CD8F}" name="Opcode " dataDxfId="3"/>
-    <tableColumn id="2" xr3:uid="{94AD8F24-8B7B-488A-B2A5-515BD41E7F08}" name="Name " dataDxfId="2"/>
-    <tableColumn id="3" xr3:uid="{F54D0553-BC6A-48B5-9E0F-A0BF767398A8}" name="Description " dataDxfId="1"/>
-    <tableColumn id="4" xr3:uid="{E6BC317F-8DC6-4A10-97A3-062D0A6033C4}" name="Operation" dataDxfId="0"/>
+    <tableColumn id="1" xr3:uid="{6F141741-2C51-4220-AFC7-E5871EC6CD8F}" name="Opcode " dataDxfId="9"/>
+    <tableColumn id="2" xr3:uid="{94AD8F24-8B7B-488A-B2A5-515BD41E7F08}" name="Name " dataDxfId="8"/>
+    <tableColumn id="3" xr3:uid="{F54D0553-BC6A-48B5-9E0F-A0BF767398A8}" name="Description " dataDxfId="7"/>
+    <tableColumn id="4" xr3:uid="{E6BC317F-8DC6-4A10-97A3-062D0A6033C4}" name="Operation" dataDxfId="6"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium2" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
 </file>
 
 <file path=xl/tables/table2.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="2" xr:uid="{151E0FC9-74A1-4492-82A5-A6974E379F5E}" name="Table2" displayName="Table2" ref="A1:D28" totalsRowShown="0" headerRowDxfId="11" dataDxfId="10">
-  <autoFilter ref="A1:D28" xr:uid="{151E0FC9-74A1-4492-82A5-A6974E379F5E}"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="2" xr:uid="{151E0FC9-74A1-4492-82A5-A6974E379F5E}" name="Table2" displayName="Table2" ref="A1:D26" totalsRowShown="0" headerRowDxfId="5" dataDxfId="4">
+  <autoFilter ref="A1:D26" xr:uid="{151E0FC9-74A1-4492-82A5-A6974E379F5E}"/>
   <tableColumns count="4">
-    <tableColumn id="1" xr3:uid="{CD4B495D-BEBD-4687-9E48-13E31F1A5458}" name="Funct " dataDxfId="9"/>
-    <tableColumn id="2" xr3:uid="{E7F73B4A-D35B-4A89-BCB0-DFA47DFF3033}" name="Name " dataDxfId="8"/>
-    <tableColumn id="3" xr3:uid="{87DDDCA8-8D3D-45D9-835E-8024A1DEE513}" name="Description " dataDxfId="7"/>
-    <tableColumn id="4" xr3:uid="{1A74FB59-C961-44A8-A91C-BB37DF112620}" name="Operation" dataDxfId="6"/>
+    <tableColumn id="1" xr3:uid="{CD4B495D-BEBD-4687-9E48-13E31F1A5458}" name="Funct " dataDxfId="3"/>
+    <tableColumn id="2" xr3:uid="{E7F73B4A-D35B-4A89-BCB0-DFA47DFF3033}" name="Name " dataDxfId="2"/>
+    <tableColumn id="3" xr3:uid="{87DDDCA8-8D3D-45D9-835E-8024A1DEE513}" name="Description " dataDxfId="1"/>
+    <tableColumn id="4" xr3:uid="{1A74FB59-C961-44A8-A91C-BB37DF112620}" name="Operation" dataDxfId="0"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium2" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
@@ -1757,10 +1736,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{8344681D-13F5-4AA9-8C1C-9376E6ED3191}">
-  <dimension ref="A1:D28"/>
+  <dimension ref="A1:D26"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A23" zoomScale="145" zoomScaleNormal="145" workbookViewId="0">
-      <selection activeCell="D14" sqref="D14"/>
+    <sheetView tabSelected="1" zoomScale="145" zoomScaleNormal="145" workbookViewId="0">
+      <selection activeCell="E12" sqref="E12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -1899,268 +1878,240 @@
       </c>
     </row>
     <row r="10" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A10" s="8" t="s">
-        <v>219</v>
-      </c>
-      <c r="B10" s="8" t="s">
-        <v>220</v>
-      </c>
-      <c r="C10" s="8" t="s">
-        <v>221</v>
-      </c>
-      <c r="D10" s="8" t="s">
-        <v>222</v>
+      <c r="A10" s="1" t="s">
+        <v>62</v>
+      </c>
+      <c r="B10" s="1" t="s">
+        <v>126</v>
+      </c>
+      <c r="C10" s="1" t="s">
+        <v>127</v>
+      </c>
+      <c r="D10" s="1" t="s">
+        <v>128</v>
       </c>
     </row>
     <row r="11" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A11" s="8" t="s">
-        <v>223</v>
-      </c>
-      <c r="B11" s="8" t="s">
-        <v>224</v>
-      </c>
-      <c r="C11" s="8" t="s">
-        <v>224</v>
-      </c>
-      <c r="D11" s="8" t="s">
-        <v>225</v>
+      <c r="A11" s="1" t="s">
+        <v>129</v>
+      </c>
+      <c r="B11" s="1" t="s">
+        <v>130</v>
+      </c>
+      <c r="C11" s="1" t="s">
+        <v>131</v>
+      </c>
+      <c r="D11" s="1" t="s">
+        <v>132</v>
       </c>
     </row>
     <row r="12" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A12" s="1" t="s">
-        <v>62</v>
+        <v>133</v>
       </c>
       <c r="B12" s="1" t="s">
-        <v>126</v>
+        <v>134</v>
       </c>
       <c r="C12" s="1" t="s">
-        <v>127</v>
+        <v>135</v>
       </c>
       <c r="D12" s="1" t="s">
-        <v>128</v>
+        <v>136</v>
       </c>
     </row>
     <row r="13" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A13" s="1" t="s">
-        <v>129</v>
+        <v>137</v>
       </c>
       <c r="B13" s="1" t="s">
-        <v>130</v>
+        <v>138</v>
       </c>
       <c r="C13" s="1" t="s">
-        <v>131</v>
+        <v>139</v>
       </c>
       <c r="D13" s="1" t="s">
-        <v>132</v>
+        <v>140</v>
       </c>
     </row>
     <row r="14" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A14" s="1" t="s">
-        <v>133</v>
+        <v>141</v>
       </c>
       <c r="B14" s="1" t="s">
-        <v>134</v>
+        <v>142</v>
       </c>
       <c r="C14" s="1" t="s">
-        <v>135</v>
+        <v>143</v>
       </c>
       <c r="D14" s="1" t="s">
-        <v>136</v>
-      </c>
-    </row>
-    <row r="15" spans="1:4" x14ac:dyDescent="0.3">
+        <v>140</v>
+      </c>
+    </row>
+    <row r="15" spans="1:4" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A15" s="1" t="s">
-        <v>137</v>
+        <v>144</v>
       </c>
       <c r="B15" s="1" t="s">
-        <v>138</v>
+        <v>145</v>
       </c>
       <c r="C15" s="1" t="s">
-        <v>139</v>
-      </c>
-      <c r="D15" s="1" t="s">
-        <v>140</v>
-      </c>
-    </row>
-    <row r="16" spans="1:4" x14ac:dyDescent="0.3">
+        <v>146</v>
+      </c>
+      <c r="D15" s="2" t="s">
+        <v>183</v>
+      </c>
+    </row>
+    <row r="16" spans="1:4" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A16" s="1" t="s">
-        <v>141</v>
+        <v>147</v>
       </c>
       <c r="B16" s="1" t="s">
-        <v>142</v>
+        <v>148</v>
       </c>
       <c r="C16" s="1" t="s">
-        <v>143</v>
-      </c>
-      <c r="D16" s="1" t="s">
-        <v>140</v>
-      </c>
-    </row>
-    <row r="17" spans="1:4" ht="28.8" x14ac:dyDescent="0.3">
+        <v>149</v>
+      </c>
+      <c r="D16" s="2" t="s">
+        <v>183</v>
+      </c>
+    </row>
+    <row r="17" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A17" s="1" t="s">
-        <v>144</v>
+        <v>66</v>
       </c>
       <c r="B17" s="1" t="s">
-        <v>145</v>
+        <v>150</v>
       </c>
       <c r="C17" s="1" t="s">
-        <v>146</v>
-      </c>
-      <c r="D17" s="2" t="s">
-        <v>183</v>
-      </c>
-    </row>
-    <row r="18" spans="1:4" ht="28.8" x14ac:dyDescent="0.3">
+        <v>151</v>
+      </c>
+      <c r="D17" s="1" t="s">
+        <v>152</v>
+      </c>
+    </row>
+    <row r="18" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A18" s="1" t="s">
-        <v>147</v>
+        <v>70</v>
       </c>
       <c r="B18" s="1" t="s">
-        <v>148</v>
+        <v>153</v>
       </c>
       <c r="C18" s="1" t="s">
-        <v>149</v>
-      </c>
-      <c r="D18" s="2" t="s">
-        <v>183</v>
+        <v>154</v>
+      </c>
+      <c r="D18" s="1" t="s">
+        <v>152</v>
       </c>
     </row>
     <row r="19" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A19" s="1" t="s">
-        <v>66</v>
+        <v>155</v>
       </c>
       <c r="B19" s="1" t="s">
-        <v>150</v>
+        <v>156</v>
       </c>
       <c r="C19" s="1" t="s">
-        <v>151</v>
+        <v>157</v>
       </c>
       <c r="D19" s="1" t="s">
-        <v>152</v>
+        <v>158</v>
       </c>
     </row>
     <row r="20" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A20" s="1" t="s">
-        <v>70</v>
+        <v>74</v>
       </c>
       <c r="B20" s="1" t="s">
-        <v>153</v>
+        <v>159</v>
       </c>
       <c r="C20" s="1" t="s">
-        <v>154</v>
+        <v>160</v>
       </c>
       <c r="D20" s="1" t="s">
-        <v>152</v>
+        <v>158</v>
       </c>
     </row>
     <row r="21" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A21" s="1" t="s">
-        <v>155</v>
+        <v>78</v>
       </c>
       <c r="B21" s="1" t="s">
-        <v>156</v>
+        <v>161</v>
       </c>
       <c r="C21" s="1" t="s">
-        <v>157</v>
+        <v>162</v>
       </c>
       <c r="D21" s="1" t="s">
-        <v>158</v>
+        <v>163</v>
       </c>
     </row>
     <row r="22" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A22" s="1" t="s">
-        <v>74</v>
+        <v>82</v>
       </c>
       <c r="B22" s="1" t="s">
-        <v>159</v>
+        <v>164</v>
       </c>
       <c r="C22" s="1" t="s">
-        <v>160</v>
+        <v>165</v>
       </c>
       <c r="D22" s="1" t="s">
-        <v>158</v>
+        <v>166</v>
       </c>
     </row>
     <row r="23" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A23" s="1" t="s">
-        <v>78</v>
+        <v>167</v>
       </c>
       <c r="B23" s="1" t="s">
-        <v>161</v>
+        <v>168</v>
       </c>
       <c r="C23" s="1" t="s">
-        <v>162</v>
+        <v>169</v>
       </c>
       <c r="D23" s="1" t="s">
-        <v>163</v>
+        <v>170</v>
       </c>
     </row>
     <row r="24" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A24" s="1" t="s">
-        <v>82</v>
+        <v>171</v>
       </c>
       <c r="B24" s="1" t="s">
-        <v>164</v>
+        <v>172</v>
       </c>
       <c r="C24" s="1" t="s">
-        <v>165</v>
+        <v>173</v>
       </c>
       <c r="D24" s="1" t="s">
-        <v>166</v>
+        <v>174</v>
       </c>
     </row>
     <row r="25" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A25" s="1" t="s">
-        <v>167</v>
+        <v>175</v>
       </c>
       <c r="B25" s="1" t="s">
-        <v>168</v>
+        <v>176</v>
       </c>
       <c r="C25" s="1" t="s">
-        <v>169</v>
+        <v>177</v>
       </c>
       <c r="D25" s="1" t="s">
-        <v>170</v>
+        <v>178</v>
       </c>
     </row>
     <row r="26" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A26" s="1" t="s">
-        <v>171</v>
+        <v>99</v>
       </c>
       <c r="B26" s="1" t="s">
-        <v>172</v>
+        <v>179</v>
       </c>
       <c r="C26" s="1" t="s">
-        <v>173</v>
+        <v>180</v>
       </c>
       <c r="D26" s="1" t="s">
-        <v>174</v>
-      </c>
-    </row>
-    <row r="27" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A27" s="1" t="s">
-        <v>175</v>
-      </c>
-      <c r="B27" s="1" t="s">
-        <v>176</v>
-      </c>
-      <c r="C27" s="1" t="s">
-        <v>177</v>
-      </c>
-      <c r="D27" s="1" t="s">
-        <v>178</v>
-      </c>
-    </row>
-    <row r="28" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A28" s="1" t="s">
-        <v>99</v>
-      </c>
-      <c r="B28" s="1" t="s">
-        <v>179</v>
-      </c>
-      <c r="C28" s="1" t="s">
-        <v>180</v>
-      </c>
-      <c r="D28" s="1" t="s">
         <v>178</v>
       </c>
     </row>

</xml_diff>